<commit_message>
update and fix test data
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-self-summary-with-xlsx-output/output/model_comparison_model_summary.xlsx
+++ b/tests/data/experiments/lr-self-summary-with-xlsx-output/output/model_comparison_model_summary.xlsx
@@ -461,15 +461,11 @@
           <t>lr_subgroups</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="B2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -488,15 +484,11 @@
           <t>lr_subgroups</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="B3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -515,15 +507,11 @@
           <t>lr_subgroups</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="B4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>

</xml_diff>